<commit_message>
formatted datasheets for readability
</commit_message>
<xml_diff>
--- a/exp 2 df input.xlsx
+++ b/exp 2 df input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce188bf86570271f/Documents/YEAR 3/Structural Mechanics and Dynamics 3/Structural Mechanics Lab Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce188bf86570271f/Documents/GitHub/SMD3-Structures-Lab-Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{212A0C10-9952-4EE0-AAE6-6EADC2DBC061}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C59CB38-48B9-4236-8B03-6A38151456D8}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,41 +44,40 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>H_D 1</t>
-  </si>
-  <si>
-    <t>H_D 2</t>
-  </si>
-  <si>
-    <t>Mean H_D</t>
-  </si>
-  <si>
-    <t>V_D 1</t>
-  </si>
-  <si>
-    <t>V_D 2</t>
-  </si>
-  <si>
-    <t>Mean V_D</t>
-  </si>
-  <si>
-    <t>Error in Weight</t>
-  </si>
-  <si>
-    <t>Error in H_D</t>
-  </si>
-  <si>
-    <t>Error in V_D</t>
+    <t>H_D 1 (m)</t>
+  </si>
+  <si>
+    <t>H_D 2 (m)</t>
+  </si>
+  <si>
+    <t>Mean H_D (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V_D 1 (m) </t>
+  </si>
+  <si>
+    <t>V_D 2 (m)</t>
+  </si>
+  <si>
+    <t>Mean V_D (m)</t>
+  </si>
+  <si>
+    <t>Error in Weight (m)</t>
+  </si>
+  <si>
+    <t>Error in H_D (m)</t>
+  </si>
+  <si>
+    <t>Error in V_D (m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,17 +108,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -132,8 +167,36 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E435CE1C-F989-4FC0-8A09-3824A70DB224}" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:K7" xr:uid="{E435CE1C-F989-4FC0-8A09-3824A70DB224}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{AC23A5CE-F338-41B2-BE43-83F722BB60F0}" name="Offset Weight (N)" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{A7549B9D-3A9E-487F-8212-6391FF1BC30F}" name="Weight" dataDxfId="10">
+      <calculatedColumnFormula>A2+9.81*0.1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{051571F2-C33F-46A4-8B89-3E506DA18C42}" name="H_D 1 (m)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{4B69CF42-EAB1-45E0-8B86-004FFD0848E9}" name="H_D 2 (m)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E121FF64-7961-42E5-89ED-2EAA01D4BCE9}" name="Mean H_D (m)" dataDxfId="7">
+      <calculatedColumnFormula>AVERAGE(C2:D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C2CE9B89-16FE-4608-A2D1-E9351BD76DD3}" name="V_D 1 (m) " dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{A0A323B8-F368-44CC-8DB4-0E8EF28C823C}" name="V_D 2 (m)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{696EE1B7-610E-4291-94FC-549303D561A0}" name="Mean V_D (m)" dataDxfId="4">
+      <calculatedColumnFormula>(F2+G2)/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{A244E44C-71A4-4D3B-89BD-D5A9D014759F}" name="Error in Weight (m)" dataDxfId="3">
+      <calculatedColumnFormula>(0.001/0.1 * 0.981)/B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{896A03F5-F023-4636-9CDC-8871965A9F2F}" name="Error in H_D (m)" dataDxfId="2">
+      <calculatedColumnFormula>ABS(D2-C2)/(2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{B4021A6C-84B1-49FB-A7D0-870ECA81D8ED}" name="Error in V_D (m)" dataDxfId="1">
+      <calculatedColumnFormula>ABS(G2-F2)/(2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,24 +516,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
@@ -481,31 +544,31 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -516,33 +579,33 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>-1.4999999999999999E-4</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <f>AVERAGE(C2:D2)</f>
         <v>-6.4999999999999994E-5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>-5.0000000000000002E-5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <f>F2+G2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>0</v>
       </c>
       <c r="J2" s="3">
         <v>0</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -554,23 +617,23 @@
         <f>A3+9.81*0.1</f>
         <v>2.9809999999999999</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>7.1000000000000002E-4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>1.33E-3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <f t="shared" ref="E3:E7" si="0">AVERAGE(C3:D3)</f>
         <v>1.0200000000000001E-3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>6.7000000000000002E-4</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>1.0499999999999999E-3</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <f>(F3+G3)/2</f>
         <v>8.5999999999999998E-4</v>
       </c>
@@ -578,11 +641,11 @@
         <f>(0.001/0.1 * 0.981)/B3</f>
         <v>3.290841999329084E-3</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <f>ABS(D3-C3)/(2)</f>
         <v>3.1E-4</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <f>ABS(G3-F3)/(2)</f>
         <v>1.8999999999999996E-4</v>
       </c>
@@ -595,23 +658,23 @@
         <f t="shared" ref="B4:B7" si="1">A4+9.81*0.1</f>
         <v>4.9809999999999999</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>2.0799999999999998E-3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>2.4199999999999998E-3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>2.2499999999999998E-3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>1.7700000000000001E-3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>1.9499999999999999E-3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <f t="shared" ref="H4:H7" si="2">(F4+G4)/2</f>
         <v>1.8600000000000001E-3</v>
       </c>
@@ -619,11 +682,11 @@
         <f>(0.001/0.1 * 0.981)/B4</f>
         <v>1.9694840393495281E-3</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <f t="shared" ref="J4:J7" si="3">ABS(D4-C4)/(2)</f>
         <v>1.7000000000000001E-4</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <f t="shared" ref="K4:K7" si="4">ABS(G4-F4)/(2)</f>
         <v>8.9999999999999911E-5</v>
       </c>
@@ -636,23 +699,23 @@
         <f t="shared" si="1"/>
         <v>6.9809999999999999</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>3.0799999999999998E-3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>3.7699999999999999E-3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>3.4250000000000001E-3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>2.64E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>3.0200000000000001E-3</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <f t="shared" si="2"/>
         <v>2.8300000000000001E-3</v>
       </c>
@@ -660,11 +723,11 @@
         <f>(0.001/0.1 * 0.981)/B5</f>
         <v>1.4052428018908466E-3</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <f t="shared" si="3"/>
         <v>3.4500000000000004E-4</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <f t="shared" si="4"/>
         <v>1.9000000000000006E-4</v>
       </c>
@@ -677,23 +740,23 @@
         <f t="shared" si="1"/>
         <v>8.9809999999999999</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>4.1700000000000001E-3</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>5.0600000000000003E-3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>4.6150000000000002E-3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>3.5500000000000002E-3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>4.0400000000000002E-3</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <f t="shared" si="2"/>
         <v>3.7950000000000002E-3</v>
       </c>
@@ -701,11 +764,11 @@
         <f>(0.001/0.1 * 0.981)/B6</f>
         <v>1.0923059792896114E-3</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <f t="shared" si="3"/>
         <v>4.4500000000000008E-4</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <f t="shared" si="4"/>
         <v>2.4499999999999999E-4</v>
       </c>
@@ -718,23 +781,23 @@
         <f t="shared" si="1"/>
         <v>10.805</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>5.45E-3</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>5.3800000000000002E-3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>5.4149999999999997E-3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>4.5100000000000001E-3</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <f t="shared" si="2"/>
         <v>4.5050000000000003E-3</v>
       </c>
@@ -742,19 +805,19 @@
         <f>(0.001/0.1 * 0.981)/B7</f>
         <v>9.0791300323924101E-4</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <f t="shared" si="3"/>
         <v>3.4999999999999875E-5</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <f t="shared" si="4"/>
         <v>5.00000000000023E-6</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>